<commit_message>
adjusted cumualtive rain and water budget figures
</commit_message>
<xml_diff>
--- a/cum_rain.xlsx
+++ b/cum_rain.xlsx
@@ -13,6 +13,20 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Cumulative.rainfall.cm</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,8 +60,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,7 +112,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$36</c:f>
+              <c:f>Sheet1!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -205,7 +220,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$36</c:f>
+              <c:f>Sheet1!$C$2:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -300,10 +315,10 @@
                   <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9.9</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9.9</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>18.899999999999999</c:v>
@@ -321,11 +336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64739968"/>
-        <c:axId val="64738432"/>
+        <c:axId val="199389568"/>
+        <c:axId val="199391104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64739968"/>
+        <c:axId val="199389568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,12 +350,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64738432"/>
+        <c:crossAx val="199391104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64738432"/>
+        <c:axId val="199391104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,7 +365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64739968"/>
+        <c:crossAx val="199389568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -694,275 +709,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:F36"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>42325</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>42326</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="C3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D6">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>42327</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="C4">
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D7">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>42328</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="F7">
+      <c r="C5">
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D8">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>42329</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="C6">
         <v>1.8</v>
       </c>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D9">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>42330</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="F9">
+      <c r="C7">
         <v>2.7</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D10">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>42331</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="F10">
+      <c r="C8">
         <v>2.7</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D11">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>42332</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="F11">
+      <c r="C9">
         <v>2.7</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D12">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>42333</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="F12">
+      <c r="C10">
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D13">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>42334</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="F13">
+      <c r="C11">
         <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D14">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>42335</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="F14">
+      <c r="C12">
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>42336</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="F15">
+      <c r="C13">
         <v>4.5</v>
       </c>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D16">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>42337</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="F16">
+      <c r="C14">
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D17">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="F17">
+      <c r="C15">
         <v>4.5</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D18">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="F18">
+      <c r="C16">
         <v>5.4</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D19">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>42340</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="F19">
+      <c r="C17">
         <v>5.4</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D20">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>42341</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="F20">
+      <c r="C18">
         <v>5.4</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D21">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>42342</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="F21">
+      <c r="C19">
         <v>6.3</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D22">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>42343</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="F22">
+      <c r="C20">
         <v>6.3</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D23">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>42344</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="F23">
+      <c r="C21">
         <v>6.3</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D24">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>42345</v>
+      </c>
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="F24">
+      <c r="C22">
         <v>7.2</v>
       </c>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>42346</v>
+      </c>
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="F25">
+      <c r="C23">
         <v>7.2</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D26">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>42347</v>
+      </c>
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="F26">
+      <c r="C24">
         <v>7.2</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D27">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>42348</v>
+      </c>
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="F27">
+      <c r="C25">
         <v>8.1</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D28">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>42349</v>
+      </c>
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="F28">
+      <c r="C26">
         <v>8.1</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D29">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>42350</v>
+      </c>
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="F29">
+      <c r="C27">
         <v>8.1</v>
       </c>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D30">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>42351</v>
+      </c>
+      <c r="B28">
         <v>27</v>
       </c>
-      <c r="F30">
+      <c r="C28">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D31">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>42352</v>
+      </c>
+      <c r="B29">
         <v>28</v>
       </c>
-      <c r="F31">
+      <c r="C29">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D32">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>42353</v>
+      </c>
+      <c r="B30">
         <v>29</v>
       </c>
-      <c r="F32">
+      <c r="C30">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D33">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>42354</v>
+      </c>
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="F33">
+      <c r="C31">
         <v>9.9</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D34">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>42355</v>
+      </c>
+      <c r="B32">
         <v>31</v>
       </c>
-      <c r="F34">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D35">
+      <c r="C32">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>42356</v>
+      </c>
+      <c r="B33">
         <v>32</v>
       </c>
-      <c r="F35">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D36">
+      <c r="C33">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>42357</v>
+      </c>
+      <c r="B34">
         <v>33</v>
       </c>
-      <c r="F36">
+      <c r="C34">
         <v>18.899999999999999</v>
       </c>
     </row>

</xml_diff>